<commit_message>
Partial Mantel tests for combined populations 1 and 2
</commit_message>
<xml_diff>
--- a/Data/PRBI_AvgLatLong.xlsx
+++ b/Data/PRBI_AvgLatLong.xlsx
@@ -1,22 +1,33 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="26812"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24131"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kyrafitz/Documents/GitHub/Premnas-biaculeatus/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kyras\OneDrive\Documents\GitHub\Premnas-biaculeatus\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD427C53-945E-47D4-BF53-2B11EBF1E0FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="35380" yWindow="460" windowWidth="25900" windowHeight="18860" tabRatio="500"/>
+    <workbookView xWindow="1680" yWindow="108" windowWidth="19656" windowHeight="11796" tabRatio="500" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Lat Long by Individual" sheetId="2" r:id="rId1"/>
     <sheet name="PRBI_AvgLatLong" sheetId="1" r:id="rId2"/>
+    <sheet name="PRBI_Comb12_AvgLatLong" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="0" concurrentCalc="0"/>
+  <calcPr calcId="191029"/>
   <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -25,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="170">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="174" uniqueCount="171">
   <si>
     <t>Population</t>
   </si>
@@ -535,12 +546,15 @@
   </si>
   <si>
     <t>Leaving out PRBI 164</t>
+  </si>
+  <si>
+    <t>1_2</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -581,6 +595,9 @@
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
     </ext>
   </extLst>
 </styleSheet>
@@ -848,22 +865,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H171"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="E28" sqref="E28"/>
+    <sheetView topLeftCell="B104" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="F109" sqref="F109"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="19.1640625" customWidth="1"/>
-    <col min="4" max="4" width="18.1640625" customWidth="1"/>
+    <col min="3" max="3" width="19.19921875" customWidth="1"/>
+    <col min="4" max="4" width="18.19921875" customWidth="1"/>
     <col min="5" max="5" width="27.5" customWidth="1"/>
-    <col min="6" max="6" width="23.6640625" customWidth="1"/>
+    <col min="6" max="6" width="23.69921875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>3</v>
       </c>
@@ -886,7 +903,7 @@
         <v>168</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>5</v>
       </c>
@@ -908,7 +925,7 @@
         <v>123.3179946125</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>6</v>
       </c>
@@ -922,7 +939,7 @@
         <v>123.3158979</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>7</v>
       </c>
@@ -936,7 +953,7 @@
         <v>123.3158979</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>8</v>
       </c>
@@ -950,7 +967,7 @@
         <v>123.32882499999999</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>9</v>
       </c>
@@ -964,7 +981,7 @@
         <v>123.32882499999999</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>10</v>
       </c>
@@ -978,7 +995,7 @@
         <v>123.3084444</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>11</v>
       </c>
@@ -992,7 +1009,7 @@
         <v>123.3084444</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>12</v>
       </c>
@@ -1006,7 +1023,7 @@
         <v>123.3086474</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>13</v>
       </c>
@@ -1020,7 +1037,7 @@
         <v>123.3097568</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>14</v>
       </c>
@@ -1034,7 +1051,7 @@
         <v>123.3097568</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>15</v>
       </c>
@@ -1048,7 +1065,7 @@
         <v>123.31031110000001</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>16</v>
       </c>
@@ -1062,7 +1079,7 @@
         <v>123.3118528</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>17</v>
       </c>
@@ -1076,7 +1093,7 @@
         <v>123.31293410000001</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>18</v>
       </c>
@@ -1090,7 +1107,7 @@
         <v>123.3132308</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>19</v>
       </c>
@@ -1104,7 +1121,7 @@
         <v>123.3469192</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>20</v>
       </c>
@@ -1118,7 +1135,7 @@
         <v>123.34559710000001</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>21</v>
       </c>
@@ -1140,7 +1157,7 @@
         <v>123.47946155000001</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>22</v>
       </c>
@@ -1154,7 +1171,7 @@
         <v>123.4851389</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>23</v>
       </c>
@@ -1168,7 +1185,7 @@
         <v>123.4877735</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>24</v>
       </c>
@@ -1182,7 +1199,7 @@
         <v>123.4900545</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>25</v>
       </c>
@@ -1196,7 +1213,7 @@
         <v>123.4900545</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>26</v>
       </c>
@@ -1210,7 +1227,7 @@
         <v>123.4736966</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>27</v>
       </c>
@@ -1224,7 +1241,7 @@
         <v>123.4743452</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>28</v>
       </c>
@@ -1238,7 +1255,7 @@
         <v>123.4743452</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>29</v>
       </c>
@@ -1252,7 +1269,7 @@
         <v>123.47457780000001</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>30</v>
       </c>
@@ -1266,7 +1283,7 @@
         <v>123.47457780000001</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>31</v>
       </c>
@@ -1280,7 +1297,7 @@
         <v>123.47766180000001</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>32</v>
       </c>
@@ -1294,7 +1311,7 @@
         <v>123.47766180000001</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>33</v>
       </c>
@@ -1308,7 +1325,7 @@
         <v>123.4774901</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>34</v>
       </c>
@@ -1322,7 +1339,7 @@
         <v>123.477198</v>
       </c>
     </row>
-    <row r="33" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>35</v>
       </c>
@@ -1336,7 +1353,7 @@
         <v>123.4758351</v>
       </c>
     </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>36</v>
       </c>
@@ -1350,7 +1367,7 @@
         <v>123.4758351</v>
       </c>
     </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>37</v>
       </c>
@@ -1372,7 +1389,7 @@
         <v>123.57853247058823</v>
       </c>
     </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>38</v>
       </c>
@@ -1386,7 +1403,7 @@
         <v>123.56904969999999</v>
       </c>
     </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>39</v>
       </c>
@@ -1400,7 +1417,7 @@
         <v>123.5691369</v>
       </c>
     </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>40</v>
       </c>
@@ -1414,7 +1431,7 @@
         <v>123.5691369</v>
       </c>
     </row>
-    <row r="40" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>41</v>
       </c>
@@ -1428,7 +1445,7 @@
         <v>123.5689489</v>
       </c>
     </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>42</v>
       </c>
@@ -1442,7 +1459,7 @@
         <v>123.5684931</v>
       </c>
     </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>43</v>
       </c>
@@ -1456,7 +1473,7 @@
         <v>123.5685467</v>
       </c>
     </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>44</v>
       </c>
@@ -1470,7 +1487,7 @@
         <v>123.5685467</v>
       </c>
     </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>45</v>
       </c>
@@ -1484,7 +1501,7 @@
         <v>123.5688171</v>
       </c>
     </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>46</v>
       </c>
@@ -1498,7 +1515,7 @@
         <v>123.5688171</v>
       </c>
     </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A46" t="s">
         <v>47</v>
       </c>
@@ -1512,7 +1529,7 @@
         <v>123.5688171</v>
       </c>
     </row>
-    <row r="47" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A47" t="s">
         <v>48</v>
       </c>
@@ -1526,7 +1543,7 @@
         <v>123.5682753</v>
       </c>
     </row>
-    <row r="48" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A48" t="s">
         <v>49</v>
       </c>
@@ -1540,7 +1557,7 @@
         <v>123.5682753</v>
       </c>
     </row>
-    <row r="49" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A49" t="s">
         <v>50</v>
       </c>
@@ -1554,7 +1571,7 @@
         <v>123.6083235</v>
       </c>
     </row>
-    <row r="50" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A50" t="s">
         <v>51</v>
       </c>
@@ -1568,7 +1585,7 @@
         <v>123.6083235</v>
       </c>
     </row>
-    <row r="51" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A51" t="s">
         <v>52</v>
       </c>
@@ -1582,7 +1599,7 @@
         <v>123.6020699</v>
       </c>
     </row>
-    <row r="52" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A52" t="s">
         <v>53</v>
       </c>
@@ -1596,7 +1613,7 @@
         <v>123.6020699</v>
       </c>
     </row>
-    <row r="54" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A54" t="s">
         <v>54</v>
       </c>
@@ -1618,7 +1635,7 @@
         <v>123.65455709999999</v>
       </c>
     </row>
-    <row r="55" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
         <v>55</v>
       </c>
@@ -1632,7 +1649,7 @@
         <v>123.64136670000001</v>
       </c>
     </row>
-    <row r="56" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
         <v>56</v>
       </c>
@@ -1646,7 +1663,7 @@
         <v>123.64136670000001</v>
       </c>
     </row>
-    <row r="57" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A57" t="s">
         <v>57</v>
       </c>
@@ -1660,7 +1677,7 @@
         <v>123.64136670000001</v>
       </c>
     </row>
-    <row r="58" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A58" t="s">
         <v>58</v>
       </c>
@@ -1674,7 +1691,7 @@
         <v>123.64136670000001</v>
       </c>
     </row>
-    <row r="59" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A59" t="s">
         <v>59</v>
       </c>
@@ -1688,7 +1705,7 @@
         <v>123.64136670000001</v>
       </c>
     </row>
-    <row r="60" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A60" t="s">
         <v>60</v>
       </c>
@@ -1702,7 +1719,7 @@
         <v>123.64136670000001</v>
       </c>
     </row>
-    <row r="61" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A61" t="s">
         <v>61</v>
       </c>
@@ -1716,7 +1733,7 @@
         <v>123.6597642</v>
       </c>
     </row>
-    <row r="62" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A62" t="s">
         <v>62</v>
       </c>
@@ -1730,7 +1747,7 @@
         <v>123.6597642</v>
       </c>
     </row>
-    <row r="63" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A63" t="s">
         <v>63</v>
       </c>
@@ -1744,7 +1761,7 @@
         <v>123.65980380000001</v>
       </c>
     </row>
-    <row r="64" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A64" t="s">
         <v>64</v>
       </c>
@@ -1758,7 +1775,7 @@
         <v>123.65980380000001</v>
       </c>
     </row>
-    <row r="65" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A65" t="s">
         <v>65</v>
       </c>
@@ -1772,7 +1789,7 @@
         <v>123.6602326</v>
       </c>
     </row>
-    <row r="66" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A66" t="s">
         <v>66</v>
       </c>
@@ -1786,7 +1803,7 @@
         <v>123.66027010000001</v>
       </c>
     </row>
-    <row r="67" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A67" t="s">
         <v>67</v>
       </c>
@@ -1800,7 +1817,7 @@
         <v>123.66027010000001</v>
       </c>
     </row>
-    <row r="68" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A68" t="s">
         <v>68</v>
       </c>
@@ -1814,7 +1831,7 @@
         <v>123.66138979999999</v>
       </c>
     </row>
-    <row r="69" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A69" t="s">
         <v>69</v>
       </c>
@@ -1828,7 +1845,7 @@
         <v>123.66225420000001</v>
       </c>
     </row>
-    <row r="70" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A70" t="s">
         <v>70</v>
       </c>
@@ -1842,7 +1859,7 @@
         <v>123.66225420000001</v>
       </c>
     </row>
-    <row r="71" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A71" t="s">
         <v>71</v>
       </c>
@@ -1856,7 +1873,7 @@
         <v>123.6623894</v>
       </c>
     </row>
-    <row r="72" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A72" t="s">
         <v>72</v>
       </c>
@@ -1870,7 +1887,7 @@
         <v>123.662621</v>
       </c>
     </row>
-    <row r="73" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A73" t="s">
         <v>73</v>
       </c>
@@ -1884,7 +1901,7 @@
         <v>123.6626574</v>
       </c>
     </row>
-    <row r="74" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A74" t="s">
         <v>74</v>
       </c>
@@ -1898,7 +1915,7 @@
         <v>123.6626574</v>
       </c>
     </row>
-    <row r="76" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A76" t="s">
         <v>75</v>
       </c>
@@ -1923,7 +1940,7 @@
         <v>169</v>
       </c>
     </row>
-    <row r="77" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A77" t="s">
         <v>76</v>
       </c>
@@ -1937,7 +1954,7 @@
         <v>123.8172369</v>
       </c>
     </row>
-    <row r="78" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A78" t="s">
         <v>77</v>
       </c>
@@ -1951,7 +1968,7 @@
         <v>123.8199307</v>
       </c>
     </row>
-    <row r="79" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A79" t="s">
         <v>78</v>
       </c>
@@ -1965,7 +1982,7 @@
         <v>123.8198529</v>
       </c>
     </row>
-    <row r="80" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A80" t="s">
         <v>79</v>
       </c>
@@ -1979,7 +1996,7 @@
         <v>123.7915878</v>
       </c>
     </row>
-    <row r="81" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A81" t="s">
         <v>80</v>
       </c>
@@ -1993,7 +2010,7 @@
         <v>123.7915878</v>
       </c>
     </row>
-    <row r="82" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A82" t="s">
         <v>81</v>
       </c>
@@ -2007,7 +2024,7 @@
         <v>123.79036360000001</v>
       </c>
     </row>
-    <row r="83" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A83" t="s">
         <v>82</v>
       </c>
@@ -2021,7 +2038,7 @@
         <v>123.78329069999999</v>
       </c>
     </row>
-    <row r="84" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A84" t="s">
         <v>83</v>
       </c>
@@ -2035,7 +2052,7 @@
         <v>123.78395</v>
       </c>
     </row>
-    <row r="85" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A85" t="s">
         <v>84</v>
       </c>
@@ -2049,7 +2066,7 @@
         <v>123.7831492</v>
       </c>
     </row>
-    <row r="86" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A86" t="s">
         <v>85</v>
       </c>
@@ -2063,7 +2080,7 @@
         <v>123.8173937</v>
       </c>
     </row>
-    <row r="87" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A87" t="s">
         <v>86</v>
       </c>
@@ -2077,7 +2094,7 @@
         <v>123.8174473</v>
       </c>
     </row>
-    <row r="88" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A88" t="s">
         <v>87</v>
       </c>
@@ -2091,7 +2108,7 @@
         <v>123.78395</v>
       </c>
     </row>
-    <row r="89" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A89" t="s">
         <v>88</v>
       </c>
@@ -2105,7 +2122,7 @@
         <v>123.8170752</v>
       </c>
     </row>
-    <row r="90" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A90" t="s">
         <v>89</v>
       </c>
@@ -2119,7 +2136,7 @@
         <v>123.8170752</v>
       </c>
     </row>
-    <row r="91" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A91" t="s">
         <v>90</v>
       </c>
@@ -2133,7 +2150,7 @@
         <v>123.8050193</v>
       </c>
     </row>
-    <row r="92" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A92" t="s">
         <v>91</v>
       </c>
@@ -2147,7 +2164,7 @@
         <v>123.8050193</v>
       </c>
     </row>
-    <row r="93" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A93" t="s">
         <v>92</v>
       </c>
@@ -2161,7 +2178,7 @@
         <v>123.8047687</v>
       </c>
     </row>
-    <row r="94" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A94" t="s">
         <v>93</v>
       </c>
@@ -2175,7 +2192,7 @@
         <v>123.8047687</v>
       </c>
     </row>
-    <row r="96" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A96" t="s">
         <v>94</v>
       </c>
@@ -2197,7 +2214,7 @@
         <v>124.0285911</v>
       </c>
     </row>
-    <row r="97" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A97" t="s">
         <v>95</v>
       </c>
@@ -2211,7 +2228,7 @@
         <v>124.0284745</v>
       </c>
     </row>
-    <row r="98" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A98" t="s">
         <v>96</v>
       </c>
@@ -2225,7 +2242,7 @@
         <v>124.0287077</v>
       </c>
     </row>
-    <row r="99" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A99" t="s">
         <v>97</v>
       </c>
@@ -2239,7 +2256,7 @@
         <v>124.0287077</v>
       </c>
     </row>
-    <row r="101" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A101" t="s">
         <v>98</v>
       </c>
@@ -2259,7 +2276,7 @@
         <v>124.0109535</v>
       </c>
     </row>
-    <row r="102" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A102" t="s">
         <v>99</v>
       </c>
@@ -2273,7 +2290,7 @@
         <v>124.0109535</v>
       </c>
     </row>
-    <row r="104" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A104" t="s">
         <v>100</v>
       </c>
@@ -2293,7 +2310,7 @@
         <v>124.032865</v>
       </c>
     </row>
-    <row r="106" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A106" t="s">
         <v>101</v>
       </c>
@@ -2315,7 +2332,7 @@
         <v>124.24895890499997</v>
       </c>
     </row>
-    <row r="107" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A107" t="s">
         <v>102</v>
       </c>
@@ -2329,7 +2346,7 @@
         <v>124.2492249</v>
       </c>
     </row>
-    <row r="108" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A108" t="s">
         <v>103</v>
       </c>
@@ -2343,7 +2360,7 @@
         <v>124.2492249</v>
       </c>
     </row>
-    <row r="109" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A109" t="s">
         <v>104</v>
       </c>
@@ -2356,8 +2373,16 @@
       <c r="D109">
         <v>124.2492099</v>
       </c>
-    </row>
-    <row r="110" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="E109">
+        <f>AVERAGE(C106:C125, C127:C147)</f>
+        <v>10.201873197560973</v>
+      </c>
+      <c r="F109">
+        <f>AVERAGE(D106:D125, D127:D147)</f>
+        <v>124.21258387560971</v>
+      </c>
+    </row>
+    <row r="110" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A110" t="s">
         <v>105</v>
       </c>
@@ -2371,7 +2396,7 @@
         <v>124.2489782</v>
       </c>
     </row>
-    <row r="111" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A111" t="s">
         <v>106</v>
       </c>
@@ -2385,7 +2410,7 @@
         <v>124.2489782</v>
       </c>
     </row>
-    <row r="112" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A112" t="s">
         <v>107</v>
       </c>
@@ -2399,7 +2424,7 @@
         <v>124.248925</v>
       </c>
     </row>
-    <row r="113" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A113" t="s">
         <v>108</v>
       </c>
@@ -2413,7 +2438,7 @@
         <v>124.2489613</v>
       </c>
     </row>
-    <row r="114" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A114" t="s">
         <v>109</v>
       </c>
@@ -2427,7 +2452,7 @@
         <v>124.2489726</v>
       </c>
     </row>
-    <row r="115" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A115" t="s">
         <v>110</v>
       </c>
@@ -2441,7 +2466,7 @@
         <v>124.2490019</v>
       </c>
     </row>
-    <row r="116" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A116" t="s">
         <v>111</v>
       </c>
@@ -2455,7 +2480,7 @@
         <v>124.2491797</v>
       </c>
     </row>
-    <row r="117" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A117" t="s">
         <v>112</v>
       </c>
@@ -2469,7 +2494,7 @@
         <v>124.2491191</v>
       </c>
     </row>
-    <row r="118" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A118" t="s">
         <v>113</v>
       </c>
@@ -2483,7 +2508,7 @@
         <v>124.24904840000001</v>
       </c>
     </row>
-    <row r="119" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A119" t="s">
         <v>114</v>
       </c>
@@ -2497,7 +2522,7 @@
         <v>124.2491191</v>
       </c>
     </row>
-    <row r="120" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A120" t="s">
         <v>115</v>
       </c>
@@ -2511,7 +2536,7 @@
         <v>124.2491191</v>
       </c>
     </row>
-    <row r="121" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A121" t="s">
         <v>116</v>
       </c>
@@ -2525,7 +2550,7 @@
         <v>124.2491191</v>
       </c>
     </row>
-    <row r="122" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A122" t="s">
         <v>117</v>
       </c>
@@ -2539,7 +2564,7 @@
         <v>124.2491191</v>
       </c>
     </row>
-    <row r="123" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A123" t="s">
         <v>118</v>
       </c>
@@ -2553,7 +2578,7 @@
         <v>124.2476369</v>
       </c>
     </row>
-    <row r="124" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A124" t="s">
         <v>119</v>
       </c>
@@ -2567,7 +2592,7 @@
         <v>124.2476369</v>
       </c>
     </row>
-    <row r="125" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A125" t="s">
         <v>120</v>
       </c>
@@ -2581,7 +2606,7 @@
         <v>124.2494847</v>
       </c>
     </row>
-    <row r="127" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A127" t="s">
         <v>121</v>
       </c>
@@ -2603,7 +2628,7 @@
         <v>124.17794099047617</v>
       </c>
     </row>
-    <row r="128" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A128" t="s">
         <v>122</v>
       </c>
@@ -2617,7 +2642,7 @@
         <v>124.177668</v>
       </c>
     </row>
-    <row r="129" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A129" t="s">
         <v>123</v>
       </c>
@@ -2631,7 +2656,7 @@
         <v>124.177668</v>
       </c>
     </row>
-    <row r="130" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A130" t="s">
         <v>124</v>
       </c>
@@ -2645,7 +2670,7 @@
         <v>124.1776984</v>
       </c>
     </row>
-    <row r="131" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A131" t="s">
         <v>125</v>
       </c>
@@ -2659,7 +2684,7 @@
         <v>124.1776794</v>
       </c>
     </row>
-    <row r="132" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A132" t="s">
         <v>126</v>
       </c>
@@ -2673,7 +2698,7 @@
         <v>124.1777245</v>
       </c>
     </row>
-    <row r="133" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A133" t="s">
         <v>127</v>
       </c>
@@ -2687,7 +2712,7 @@
         <v>124.1777495</v>
       </c>
     </row>
-    <row r="134" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A134" t="s">
         <v>128</v>
       </c>
@@ -2701,7 +2726,7 @@
         <v>124.1777495</v>
       </c>
     </row>
-    <row r="135" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A135" t="s">
         <v>129</v>
       </c>
@@ -2715,7 +2740,7 @@
         <v>124.1777914</v>
       </c>
     </row>
-    <row r="136" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A136" t="s">
         <v>130</v>
       </c>
@@ -2729,7 +2754,7 @@
         <v>124.17785809999999</v>
       </c>
     </row>
-    <row r="137" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A137" t="s">
         <v>131</v>
       </c>
@@ -2743,7 +2768,7 @@
         <v>124.1780528</v>
       </c>
     </row>
-    <row r="138" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A138" t="s">
         <v>132</v>
       </c>
@@ -2757,7 +2782,7 @@
         <v>124.1780656</v>
       </c>
     </row>
-    <row r="139" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A139" t="s">
         <v>133</v>
       </c>
@@ -2771,7 +2796,7 @@
         <v>124.178077</v>
       </c>
     </row>
-    <row r="140" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A140" t="s">
         <v>134</v>
       </c>
@@ -2785,7 +2810,7 @@
         <v>124.178077</v>
       </c>
     </row>
-    <row r="141" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A141" t="s">
         <v>135</v>
       </c>
@@ -2799,7 +2824,7 @@
         <v>124.17812910000001</v>
       </c>
     </row>
-    <row r="142" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A142" t="s">
         <v>136</v>
       </c>
@@ -2813,7 +2838,7 @@
         <v>124.17812910000001</v>
       </c>
     </row>
-    <row r="143" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A143" t="s">
         <v>137</v>
       </c>
@@ -2827,7 +2852,7 @@
         <v>124.17817239999999</v>
       </c>
     </row>
-    <row r="144" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A144" t="s">
         <v>138</v>
       </c>
@@ -2841,7 +2866,7 @@
         <v>124.17817239999999</v>
       </c>
     </row>
-    <row r="145" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A145" t="s">
         <v>139</v>
       </c>
@@ -2855,7 +2880,7 @@
         <v>124.1782157</v>
       </c>
     </row>
-    <row r="146" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A146" t="s">
         <v>140</v>
       </c>
@@ -2869,7 +2894,7 @@
         <v>124.1782157</v>
       </c>
     </row>
-    <row r="147" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A147" t="s">
         <v>141</v>
       </c>
@@ -2883,7 +2908,7 @@
         <v>124.1782357</v>
       </c>
     </row>
-    <row r="149" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A149" t="s">
         <v>142</v>
       </c>
@@ -2905,7 +2930,7 @@
         <v>125.02510148000003</v>
       </c>
     </row>
-    <row r="150" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A150" t="s">
         <v>143</v>
       </c>
@@ -2919,7 +2944,7 @@
         <v>125.0247354</v>
       </c>
     </row>
-    <row r="151" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A151" t="s">
         <v>144</v>
       </c>
@@ -2933,7 +2958,7 @@
         <v>125.0249359</v>
       </c>
     </row>
-    <row r="152" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A152" t="s">
         <v>145</v>
       </c>
@@ -2947,7 +2972,7 @@
         <v>125.0247469</v>
       </c>
     </row>
-    <row r="153" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A153" t="s">
         <v>146</v>
       </c>
@@ -2961,7 +2986,7 @@
         <v>125.0247469</v>
       </c>
     </row>
-    <row r="154" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A154" t="s">
         <v>147</v>
       </c>
@@ -2975,7 +3000,7 @@
         <v>125.0247942</v>
       </c>
     </row>
-    <row r="155" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A155" t="s">
         <v>148</v>
       </c>
@@ -2989,7 +3014,7 @@
         <v>125.0247942</v>
       </c>
     </row>
-    <row r="156" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A156" t="s">
         <v>149</v>
       </c>
@@ -3003,7 +3028,7 @@
         <v>125.0247942</v>
       </c>
     </row>
-    <row r="157" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A157" t="s">
         <v>150</v>
       </c>
@@ -3017,7 +3042,7 @@
         <v>125.02498</v>
       </c>
     </row>
-    <row r="158" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A158" t="s">
         <v>151</v>
       </c>
@@ -3031,7 +3056,7 @@
         <v>125.0252776</v>
       </c>
     </row>
-    <row r="159" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A159" t="s">
         <v>152</v>
       </c>
@@ -3045,7 +3070,7 @@
         <v>125.02532239999999</v>
       </c>
     </row>
-    <row r="160" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A160" t="s">
         <v>153</v>
       </c>
@@ -3059,7 +3084,7 @@
         <v>125.0253414</v>
       </c>
     </row>
-    <row r="161" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A161" t="s">
         <v>154</v>
       </c>
@@ -3073,7 +3098,7 @@
         <v>125.0253677</v>
       </c>
     </row>
-    <row r="162" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A162" t="s">
         <v>155</v>
       </c>
@@ -3087,7 +3112,7 @@
         <v>125.0253677</v>
       </c>
     </row>
-    <row r="163" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A163" t="s">
         <v>156</v>
       </c>
@@ -3101,7 +3126,7 @@
         <v>125.0252232</v>
       </c>
     </row>
-    <row r="164" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A164" t="s">
         <v>157</v>
       </c>
@@ -3115,7 +3140,7 @@
         <v>125.02525110000001</v>
       </c>
     </row>
-    <row r="165" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A165" t="s">
         <v>158</v>
       </c>
@@ -3129,7 +3154,7 @@
         <v>125.0252924</v>
       </c>
     </row>
-    <row r="166" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A166" t="s">
         <v>159</v>
       </c>
@@ -3143,7 +3168,7 @@
         <v>125.0252924</v>
       </c>
     </row>
-    <row r="167" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A167" t="s">
         <v>160</v>
       </c>
@@ -3157,7 +3182,7 @@
         <v>125.0254841</v>
       </c>
     </row>
-    <row r="168" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A168" t="s">
         <v>161</v>
       </c>
@@ -3171,7 +3196,7 @@
         <v>125.0255465</v>
       </c>
     </row>
-    <row r="170" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A170" t="s">
         <v>162</v>
       </c>
@@ -3191,7 +3216,7 @@
         <v>124.65605770000001</v>
       </c>
     </row>
-    <row r="171" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A171" t="s">
         <v>163</v>
       </c>
@@ -3211,20 +3236,20 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11.19921875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="18.33203125" customWidth="1"/>
-    <col min="3" max="3" width="14.83203125" customWidth="1"/>
+    <col min="2" max="2" width="18.296875" customWidth="1"/>
+    <col min="3" max="3" width="14.796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -3235,7 +3260,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -3246,7 +3271,7 @@
         <v>124.24895890000001</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -3257,7 +3282,7 @@
         <v>124.177941</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>7</v>
       </c>
@@ -3268,7 +3293,7 @@
         <v>123.31799460000001</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>8</v>
       </c>
@@ -3279,7 +3304,7 @@
         <v>123.47946159999999</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>9</v>
       </c>
@@ -3290,7 +3315,7 @@
         <v>123.57853249999999</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>10</v>
       </c>
@@ -3301,7 +3326,7 @@
         <v>123.65455710000001</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>11</v>
       </c>
@@ -3312,7 +3337,7 @@
         <v>123.80282073333332</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>13</v>
       </c>
@@ -3323,7 +3348,7 @@
         <v>124.0285911</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>14</v>
       </c>
@@ -3334,7 +3359,7 @@
         <v>124.0109535</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>15</v>
       </c>
@@ -3345,7 +3370,7 @@
         <v>124.032865</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>19</v>
       </c>
@@ -3356,7 +3381,7 @@
         <v>125.02510150000001</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>22</v>
       </c>
@@ -3365,6 +3390,114 @@
       </c>
       <c r="C13">
         <v>124.65605770000001</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F269C4CE-4124-438B-9C72-733D2BA42BD0}">
+  <dimension ref="A1:C8"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F14" sqref="F14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="15.3984375" customWidth="1"/>
+    <col min="2" max="2" width="12.19921875" customWidth="1"/>
+    <col min="3" max="3" width="18.59765625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>170</v>
+      </c>
+      <c r="B2">
+        <v>10.201873197560973</v>
+      </c>
+      <c r="C2">
+        <v>124.21258387560971</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>7</v>
+      </c>
+      <c r="B3">
+        <v>9.414770978</v>
+      </c>
+      <c r="C3">
+        <v>123.31799460000001</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>8</v>
+      </c>
+      <c r="B4">
+        <v>9.616869822</v>
+      </c>
+      <c r="C4">
+        <v>123.47946159999999</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>9</v>
+      </c>
+      <c r="B5">
+        <v>9.848377696</v>
+      </c>
+      <c r="C5">
+        <v>123.57853249999999</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>10</v>
+      </c>
+      <c r="B6">
+        <v>10.073306219999999</v>
+      </c>
+      <c r="C6">
+        <v>123.65455710000001</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>11</v>
+      </c>
+      <c r="B7">
+        <v>10.224988701111108</v>
+      </c>
+      <c r="C7">
+        <v>123.80282073333332</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>19</v>
+      </c>
+      <c r="B8">
+        <v>10.01649883</v>
+      </c>
+      <c r="C8">
+        <v>125.02510150000001</v>
       </c>
     </row>
   </sheetData>

</xml_diff>